<commit_message>
tring to improve the system
</commit_message>
<xml_diff>
--- a/weekly_menu_generator/predictions/cardapio_predito.xlsx
+++ b/weekly_menu_generator/predictions/cardapio_predito.xlsx
@@ -474,17 +474,9 @@
           <t>arroz</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>batata e cenoura</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
@@ -501,17 +493,9 @@
           <t>arroz</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>batata e cenoura</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
@@ -525,18 +509,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>arroz</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>ratatouille</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>linguiça</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>batata e cenoura</t>
+          <t>abobrinha</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -552,20 +536,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>arroz</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
+          <t>ratatouille</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>batata e cenoura</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
@@ -579,18 +555,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>arroz</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>ratatouille</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>bife de frango</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>batata e cenoura</t>
+          <t>cenoura ralada</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -606,20 +582,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>arroz</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
+          <t>ratatouille</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>batata e cenoura</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
@@ -631,20 +599,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>arroz</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>feijão</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>carne moída</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>batata e cenoura</t>
+          <t>maionese</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>

</xml_diff>

<commit_message>
network with description image
</commit_message>
<xml_diff>
--- a/weekly_menu_generator/predictions/cardapio_predito.xlsx
+++ b/weekly_menu_generator/predictions/cardapio_predito.xlsx
@@ -481,12 +481,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>kibe</t>
+          <t>fricassê</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>abobrinha com calabresa</t>
+          <t>cenoura ralada</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -510,14 +510,10 @@
           <t>feijão</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ovo frito</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>batata</t>
+          <t>batata e cenoura</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -543,12 +539,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>bife de carne moída</t>
+          <t>kibe</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>batata</t>
+          <t>batata doce</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -574,12 +570,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>bife de carne moída</t>
+          <t>frango</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>tomate</t>
+          <t>abóbora</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -605,12 +601,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>carne de porco</t>
+          <t>bife bovino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>tomate</t>
+          <t>batata e cenoura</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -626,16 +622,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Estrogonofe de frango</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+          <t>arroz</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>feijão</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>bife de frango</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>ovo cozido</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>maionese</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
@@ -659,12 +663,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>carne moída</t>
+          <t>kibe</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>batata assada</t>
+          <t>batata</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>

</xml_diff>